<commit_message>
02/01/2024 dentro do dopcumento
</commit_message>
<xml_diff>
--- a/modelo_final_v2.xlsx
+++ b/modelo_final_v2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pcp2\formatarExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A0E939-AFE0-47AE-BFCA-E0328134E0C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CFE6C58-4B04-4B0C-AFA4-447F4BC1DC3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-1575" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -691,6 +691,267 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="21" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -703,272 +964,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="21" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="10" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1333,7 +1333,7 @@
   <dimension ref="A1:AA51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A4"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1350,96 +1350,96 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19"/>
-      <c r="B1" s="22" t="s">
+      <c r="A1" s="106"/>
+      <c r="B1" s="109" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="28" t="s">
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="110" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="29"/>
+      <c r="H1" s="68"/>
       <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="20"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="28" t="s">
+      <c r="A2" s="107"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="110" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="29"/>
+      <c r="H2" s="68"/>
       <c r="I2" s="2">
-        <v>45216</v>
+        <v>45293</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="20"/>
-      <c r="B3" s="30" t="s">
+      <c r="A3" s="107"/>
+      <c r="B3" s="111" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="28" t="s">
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="29"/>
+      <c r="H3" s="68"/>
       <c r="I3" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="21"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="28" t="s">
+      <c r="A4" s="108"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="110" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="29"/>
+      <c r="H4" s="68"/>
       <c r="I4" s="4">
         <v>44197</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="31"/>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="32"/>
+      <c r="A5" s="90"/>
+      <c r="B5" s="90"/>
+      <c r="C5" s="90"/>
+      <c r="D5" s="90"/>
+      <c r="E5" s="90"/>
+      <c r="F5" s="90"/>
+      <c r="G5" s="90"/>
+      <c r="H5" s="90"/>
+      <c r="I5" s="91"/>
     </row>
     <row r="6" spans="1:27" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
       <c r="F6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="34" t="s">
+      <c r="G6" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="35"/>
-      <c r="I6" s="36"/>
+      <c r="H6" s="98"/>
+      <c r="I6" s="79"/>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
       <c r="L6" s="7"/>
@@ -1460,182 +1460,182 @@
       <c r="AA6" s="6"/>
     </row>
     <row r="7" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="99" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="99" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="37" t="s">
+      <c r="C7" s="99" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="40" t="s">
+      <c r="D7" s="102" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="38"/>
+      <c r="E7" s="100"/>
       <c r="F7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="41" t="s">
+      <c r="G7" s="92" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="42"/>
-      <c r="I7" s="43"/>
+      <c r="H7" s="93"/>
+      <c r="I7" s="94"/>
       <c r="L7" s="7"/>
     </row>
     <row r="8" spans="1:27" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="38"/>
-      <c r="B8" s="38"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
+      <c r="A8" s="100"/>
+      <c r="B8" s="100"/>
+      <c r="C8" s="101"/>
+      <c r="D8" s="100"/>
+      <c r="E8" s="100"/>
       <c r="F8" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="44" t="s">
+      <c r="G8" s="103" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="45"/>
-      <c r="I8" s="46"/>
+      <c r="H8" s="104"/>
+      <c r="I8" s="105"/>
     </row>
     <row r="9" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="47" t="s">
+      <c r="A9" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="48"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="36"/>
+      <c r="B9" s="78"/>
+      <c r="C9" s="78"/>
+      <c r="D9" s="78"/>
+      <c r="E9" s="78"/>
+      <c r="F9" s="78"/>
+      <c r="G9" s="78"/>
+      <c r="H9" s="78"/>
+      <c r="I9" s="79"/>
     </row>
     <row r="10" spans="1:27" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="49" t="s">
+      <c r="A10" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="50"/>
-      <c r="C10" s="50"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="50"/>
-      <c r="H10" s="50"/>
-      <c r="I10" s="51"/>
+      <c r="B10" s="88"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="88"/>
+      <c r="E10" s="88"/>
+      <c r="F10" s="88"/>
+      <c r="G10" s="88"/>
+      <c r="H10" s="88"/>
+      <c r="I10" s="89"/>
     </row>
     <row r="11" spans="1:27" s="9" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="50"/>
-      <c r="B11" s="50"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="50"/>
-      <c r="H11" s="50"/>
-      <c r="I11" s="51"/>
+      <c r="A11" s="88"/>
+      <c r="B11" s="88"/>
+      <c r="C11" s="88"/>
+      <c r="D11" s="88"/>
+      <c r="E11" s="88"/>
+      <c r="F11" s="88"/>
+      <c r="G11" s="88"/>
+      <c r="H11" s="88"/>
+      <c r="I11" s="89"/>
     </row>
     <row r="12" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
-      <c r="B12" s="31"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="32"/>
+      <c r="A12" s="90"/>
+      <c r="B12" s="90"/>
+      <c r="C12" s="90"/>
+      <c r="D12" s="90"/>
+      <c r="E12" s="90"/>
+      <c r="F12" s="90"/>
+      <c r="G12" s="90"/>
+      <c r="H12" s="90"/>
+      <c r="I12" s="91"/>
     </row>
     <row r="13" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="52" t="s">
+      <c r="A13" s="83" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
       <c r="F13" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="41" t="s">
+      <c r="G13" s="92" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="42"/>
-      <c r="I13" s="43"/>
+      <c r="H13" s="93"/>
+      <c r="I13" s="94"/>
     </row>
     <row r="14" spans="1:27" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="53"/>
-      <c r="B14" s="54"/>
-      <c r="C14" s="54"/>
-      <c r="D14" s="54"/>
-      <c r="E14" s="54"/>
+      <c r="A14" s="45"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
       <c r="F14" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G14" s="55" t="s">
+      <c r="G14" s="95" t="s">
         <v>18</v>
       </c>
-      <c r="H14" s="56"/>
-      <c r="I14" s="57"/>
+      <c r="H14" s="96"/>
+      <c r="I14" s="97"/>
     </row>
     <row r="15" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="47" t="s">
+      <c r="A15" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="48"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="48"/>
-      <c r="H15" s="48"/>
-      <c r="I15" s="36"/>
+      <c r="B15" s="78"/>
+      <c r="C15" s="78"/>
+      <c r="D15" s="78"/>
+      <c r="E15" s="78"/>
+      <c r="F15" s="78"/>
+      <c r="G15" s="78"/>
+      <c r="H15" s="78"/>
+      <c r="I15" s="79"/>
     </row>
     <row r="16" spans="1:27" s="9" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="49" t="s">
+      <c r="A16" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="58"/>
-      <c r="C16" s="58"/>
-      <c r="D16" s="58"/>
-      <c r="E16" s="58"/>
-      <c r="F16" s="58"/>
-      <c r="G16" s="58"/>
-      <c r="H16" s="58"/>
-      <c r="I16" s="59"/>
+      <c r="B16" s="81"/>
+      <c r="C16" s="81"/>
+      <c r="D16" s="81"/>
+      <c r="E16" s="81"/>
+      <c r="F16" s="81"/>
+      <c r="G16" s="81"/>
+      <c r="H16" s="81"/>
+      <c r="I16" s="82"/>
     </row>
     <row r="17" spans="1:27" s="9" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="58"/>
-      <c r="B17" s="58"/>
-      <c r="C17" s="58"/>
-      <c r="D17" s="58"/>
-      <c r="E17" s="58"/>
-      <c r="F17" s="58"/>
-      <c r="G17" s="58"/>
-      <c r="H17" s="58"/>
-      <c r="I17" s="59"/>
+      <c r="A17" s="81"/>
+      <c r="B17" s="81"/>
+      <c r="C17" s="81"/>
+      <c r="D17" s="81"/>
+      <c r="E17" s="81"/>
+      <c r="F17" s="81"/>
+      <c r="G17" s="81"/>
+      <c r="H17" s="81"/>
+      <c r="I17" s="82"/>
     </row>
     <row r="18" spans="1:27" s="9" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="58"/>
-      <c r="B18" s="58"/>
-      <c r="C18" s="58"/>
-      <c r="D18" s="58"/>
-      <c r="E18" s="58"/>
-      <c r="F18" s="58"/>
-      <c r="G18" s="58"/>
-      <c r="H18" s="58"/>
-      <c r="I18" s="59"/>
+      <c r="A18" s="81"/>
+      <c r="B18" s="81"/>
+      <c r="C18" s="81"/>
+      <c r="D18" s="81"/>
+      <c r="E18" s="81"/>
+      <c r="F18" s="81"/>
+      <c r="G18" s="81"/>
+      <c r="H18" s="81"/>
+      <c r="I18" s="82"/>
     </row>
     <row r="19" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="58"/>
-      <c r="B19" s="58"/>
-      <c r="C19" s="58"/>
-      <c r="D19" s="58"/>
-      <c r="E19" s="58"/>
-      <c r="F19" s="58"/>
-      <c r="G19" s="58"/>
-      <c r="H19" s="58"/>
-      <c r="I19" s="59"/>
+      <c r="A19" s="81"/>
+      <c r="B19" s="81"/>
+      <c r="C19" s="81"/>
+      <c r="D19" s="81"/>
+      <c r="E19" s="81"/>
+      <c r="F19" s="81"/>
+      <c r="G19" s="81"/>
+      <c r="H19" s="81"/>
+      <c r="I19" s="82"/>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
@@ -1656,172 +1656,172 @@
       <c r="AA19" s="6"/>
     </row>
     <row r="20" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="60"/>
-      <c r="B20" s="61"/>
-      <c r="C20" s="61"/>
-      <c r="D20" s="61"/>
-      <c r="E20" s="61"/>
-      <c r="F20" s="61"/>
-      <c r="G20" s="61"/>
-      <c r="H20" s="61"/>
-      <c r="I20" s="62"/>
+      <c r="A20" s="71"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="72"/>
     </row>
     <row r="21" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="52" t="s">
+      <c r="A21" s="83" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="23"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="63" t="s">
+      <c r="B21" s="40"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="84" t="s">
         <v>15</v>
       </c>
-      <c r="G21" s="65" t="s">
+      <c r="G21" s="86" t="s">
         <v>25</v>
       </c>
-      <c r="H21" s="66"/>
-      <c r="I21" s="66"/>
+      <c r="H21" s="87"/>
+      <c r="I21" s="87"/>
     </row>
     <row r="22" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="25"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="64"/>
-      <c r="G22" s="66"/>
-      <c r="H22" s="66"/>
-      <c r="I22" s="66"/>
+      <c r="A22" s="53"/>
+      <c r="B22" s="54"/>
+      <c r="C22" s="54"/>
+      <c r="D22" s="54"/>
+      <c r="E22" s="54"/>
+      <c r="F22" s="85"/>
+      <c r="G22" s="87"/>
+      <c r="H22" s="87"/>
+      <c r="I22" s="87"/>
     </row>
     <row r="23" spans="1:27" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="67" t="s">
+      <c r="B23" s="75" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="68"/>
-      <c r="D23" s="68"/>
-      <c r="E23" s="68"/>
-      <c r="F23" s="69"/>
-      <c r="G23" s="69"/>
-      <c r="H23" s="69"/>
-      <c r="I23" s="70"/>
+      <c r="C23" s="65"/>
+      <c r="D23" s="65"/>
+      <c r="E23" s="65"/>
+      <c r="F23" s="76"/>
+      <c r="G23" s="76"/>
+      <c r="H23" s="76"/>
+      <c r="I23" s="77"/>
     </row>
     <row r="24" spans="1:27" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="71" t="s">
+      <c r="B24" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="68"/>
-      <c r="D24" s="68"/>
-      <c r="E24" s="68"/>
-      <c r="F24" s="68"/>
-      <c r="G24" s="68"/>
-      <c r="H24" s="68"/>
-      <c r="I24" s="72"/>
+      <c r="C24" s="65"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="65"/>
+      <c r="F24" s="65"/>
+      <c r="G24" s="65"/>
+      <c r="H24" s="65"/>
+      <c r="I24" s="66"/>
     </row>
     <row r="25" spans="1:27" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="71" t="s">
+      <c r="B25" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="68"/>
-      <c r="D25" s="68"/>
-      <c r="E25" s="68"/>
-      <c r="F25" s="68"/>
-      <c r="G25" s="68"/>
-      <c r="H25" s="68"/>
-      <c r="I25" s="72"/>
+      <c r="C25" s="65"/>
+      <c r="D25" s="65"/>
+      <c r="E25" s="65"/>
+      <c r="F25" s="65"/>
+      <c r="G25" s="65"/>
+      <c r="H25" s="65"/>
+      <c r="I25" s="66"/>
     </row>
     <row r="26" spans="1:27" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="71" t="s">
+      <c r="B26" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="68"/>
-      <c r="D26" s="68"/>
-      <c r="E26" s="68"/>
-      <c r="F26" s="68"/>
-      <c r="G26" s="68"/>
-      <c r="H26" s="68"/>
-      <c r="I26" s="72"/>
+      <c r="C26" s="65"/>
+      <c r="D26" s="65"/>
+      <c r="E26" s="65"/>
+      <c r="F26" s="65"/>
+      <c r="G26" s="65"/>
+      <c r="H26" s="65"/>
+      <c r="I26" s="66"/>
     </row>
     <row r="27" spans="1:27" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="71" t="s">
+      <c r="B27" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="68"/>
-      <c r="D27" s="68"/>
-      <c r="E27" s="68"/>
-      <c r="F27" s="68"/>
-      <c r="G27" s="68"/>
-      <c r="H27" s="68"/>
-      <c r="I27" s="72"/>
+      <c r="C27" s="65"/>
+      <c r="D27" s="65"/>
+      <c r="E27" s="65"/>
+      <c r="F27" s="65"/>
+      <c r="G27" s="65"/>
+      <c r="H27" s="65"/>
+      <c r="I27" s="66"/>
     </row>
     <row r="28" spans="1:27" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B28" s="71" t="s">
+      <c r="B28" s="64" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="68"/>
-      <c r="D28" s="68"/>
-      <c r="E28" s="68"/>
-      <c r="F28" s="68"/>
-      <c r="G28" s="68"/>
-      <c r="H28" s="68"/>
-      <c r="I28" s="72"/>
+      <c r="C28" s="65"/>
+      <c r="D28" s="65"/>
+      <c r="E28" s="65"/>
+      <c r="F28" s="65"/>
+      <c r="G28" s="65"/>
+      <c r="H28" s="65"/>
+      <c r="I28" s="66"/>
     </row>
     <row r="29" spans="1:27" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="73" t="s">
+      <c r="A29" s="67" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="29"/>
-      <c r="C29" s="74" t="s">
+      <c r="B29" s="68"/>
+      <c r="C29" s="69" t="s">
         <v>39</v>
       </c>
-      <c r="D29" s="75"/>
-      <c r="E29" s="75"/>
-      <c r="F29" s="75"/>
-      <c r="G29" s="75"/>
-      <c r="H29" s="75"/>
-      <c r="I29" s="76"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="34"/>
+      <c r="H29" s="34"/>
+      <c r="I29" s="70"/>
     </row>
     <row r="30" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="60"/>
-      <c r="B30" s="61"/>
-      <c r="C30" s="61"/>
-      <c r="D30" s="61"/>
-      <c r="E30" s="61"/>
-      <c r="F30" s="61"/>
-      <c r="G30" s="61"/>
-      <c r="H30" s="61"/>
-      <c r="I30" s="62"/>
+      <c r="A30" s="71"/>
+      <c r="B30" s="43"/>
+      <c r="C30" s="43"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="43"/>
+      <c r="H30" s="43"/>
+      <c r="I30" s="72"/>
     </row>
     <row r="31" spans="1:27" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="33" t="s">
+      <c r="A31" s="73" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="23"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="23"/>
-      <c r="H31" s="23"/>
-      <c r="I31" s="77"/>
+      <c r="B31" s="40"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="40"/>
+      <c r="H31" s="40"/>
+      <c r="I31" s="74"/>
       <c r="J31" s="6"/>
       <c r="K31" s="6"/>
       <c r="L31" s="6"/>
@@ -1842,202 +1842,202 @@
       <c r="AA31" s="6"/>
     </row>
     <row r="32" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="78" t="s">
+      <c r="A32" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="B32" s="23"/>
-      <c r="C32" s="23"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="79" t="s">
+      <c r="B32" s="40"/>
+      <c r="C32" s="40"/>
+      <c r="D32" s="52"/>
+      <c r="E32" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="F32" s="78" t="s">
+      <c r="F32" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="G32" s="81"/>
-      <c r="H32" s="79" t="s">
+      <c r="G32" s="58"/>
+      <c r="H32" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="I32" s="85" t="s">
+      <c r="I32" s="62" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:27" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="25"/>
-      <c r="B33" s="26"/>
-      <c r="C33" s="26"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="80"/>
-      <c r="F33" s="82"/>
-      <c r="G33" s="83"/>
-      <c r="H33" s="84"/>
-      <c r="I33" s="86"/>
+      <c r="A33" s="53"/>
+      <c r="B33" s="54"/>
+      <c r="C33" s="54"/>
+      <c r="D33" s="55"/>
+      <c r="E33" s="57"/>
+      <c r="F33" s="59"/>
+      <c r="G33" s="60"/>
+      <c r="H33" s="61"/>
+      <c r="I33" s="63"/>
     </row>
     <row r="34" spans="1:27" s="9" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="87"/>
-      <c r="B34" s="75"/>
-      <c r="C34" s="75"/>
-      <c r="D34" s="88"/>
+      <c r="A34" s="33"/>
+      <c r="B34" s="34"/>
+      <c r="C34" s="34"/>
+      <c r="D34" s="35"/>
       <c r="E34" s="13"/>
-      <c r="F34" s="89"/>
-      <c r="G34" s="90"/>
+      <c r="F34" s="36"/>
+      <c r="G34" s="37"/>
       <c r="H34" s="14"/>
       <c r="I34" s="14"/>
     </row>
     <row r="35" spans="1:27" s="9" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="87"/>
-      <c r="B35" s="75"/>
-      <c r="C35" s="75"/>
-      <c r="D35" s="88"/>
+      <c r="A35" s="33"/>
+      <c r="B35" s="34"/>
+      <c r="C35" s="34"/>
+      <c r="D35" s="35"/>
       <c r="E35" s="13"/>
-      <c r="F35" s="89"/>
-      <c r="G35" s="90"/>
+      <c r="F35" s="36"/>
+      <c r="G35" s="37"/>
       <c r="H35" s="14"/>
       <c r="I35" s="14"/>
     </row>
     <row r="36" spans="1:27" s="9" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="87"/>
-      <c r="B36" s="75"/>
-      <c r="C36" s="75"/>
-      <c r="D36" s="88"/>
+      <c r="A36" s="33"/>
+      <c r="B36" s="34"/>
+      <c r="C36" s="34"/>
+      <c r="D36" s="35"/>
       <c r="E36" s="13"/>
-      <c r="F36" s="89"/>
-      <c r="G36" s="90"/>
+      <c r="F36" s="36"/>
+      <c r="G36" s="37"/>
       <c r="H36" s="14"/>
       <c r="I36" s="14"/>
     </row>
     <row r="37" spans="1:27" s="9" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="87"/>
-      <c r="B37" s="75"/>
-      <c r="C37" s="75"/>
-      <c r="D37" s="88"/>
+      <c r="A37" s="33"/>
+      <c r="B37" s="34"/>
+      <c r="C37" s="34"/>
+      <c r="D37" s="35"/>
       <c r="E37" s="13"/>
-      <c r="F37" s="89"/>
-      <c r="G37" s="90"/>
+      <c r="F37" s="36"/>
+      <c r="G37" s="37"/>
       <c r="H37" s="14"/>
       <c r="I37" s="14"/>
     </row>
     <row r="38" spans="1:27" s="9" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="87"/>
-      <c r="B38" s="75"/>
-      <c r="C38" s="75"/>
-      <c r="D38" s="88"/>
+      <c r="A38" s="33"/>
+      <c r="B38" s="34"/>
+      <c r="C38" s="34"/>
+      <c r="D38" s="35"/>
       <c r="E38" s="13"/>
-      <c r="F38" s="89"/>
-      <c r="G38" s="90"/>
+      <c r="F38" s="36"/>
+      <c r="G38" s="37"/>
       <c r="H38" s="14"/>
       <c r="I38" s="14"/>
     </row>
     <row r="39" spans="1:27" s="9" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="87"/>
-      <c r="B39" s="75"/>
-      <c r="C39" s="75"/>
-      <c r="D39" s="88"/>
+      <c r="A39" s="33"/>
+      <c r="B39" s="34"/>
+      <c r="C39" s="34"/>
+      <c r="D39" s="35"/>
       <c r="E39" s="13"/>
-      <c r="F39" s="89"/>
-      <c r="G39" s="90"/>
+      <c r="F39" s="36"/>
+      <c r="G39" s="37"/>
       <c r="H39" s="14"/>
       <c r="I39" s="14"/>
     </row>
     <row r="40" spans="1:27" s="9" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="87"/>
-      <c r="B40" s="75"/>
-      <c r="C40" s="75"/>
-      <c r="D40" s="88"/>
+      <c r="A40" s="33"/>
+      <c r="B40" s="34"/>
+      <c r="C40" s="34"/>
+      <c r="D40" s="35"/>
       <c r="E40" s="13"/>
-      <c r="F40" s="89"/>
-      <c r="G40" s="90"/>
+      <c r="F40" s="36"/>
+      <c r="G40" s="37"/>
       <c r="H40" s="14"/>
       <c r="I40" s="14"/>
     </row>
     <row r="41" spans="1:27" s="9" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="87"/>
-      <c r="B41" s="75"/>
-      <c r="C41" s="75"/>
-      <c r="D41" s="88"/>
+      <c r="A41" s="33"/>
+      <c r="B41" s="34"/>
+      <c r="C41" s="34"/>
+      <c r="D41" s="35"/>
       <c r="E41" s="13"/>
-      <c r="F41" s="89"/>
-      <c r="G41" s="90"/>
+      <c r="F41" s="36"/>
+      <c r="G41" s="37"/>
       <c r="H41" s="14"/>
       <c r="I41" s="14"/>
     </row>
     <row r="42" spans="1:27" s="9" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="87"/>
-      <c r="B42" s="75"/>
-      <c r="C42" s="75"/>
-      <c r="D42" s="88"/>
+      <c r="A42" s="33"/>
+      <c r="B42" s="34"/>
+      <c r="C42" s="34"/>
+      <c r="D42" s="35"/>
       <c r="E42" s="13"/>
-      <c r="F42" s="89"/>
-      <c r="G42" s="90"/>
+      <c r="F42" s="36"/>
+      <c r="G42" s="37"/>
       <c r="H42" s="14"/>
       <c r="I42" s="14"/>
     </row>
     <row r="43" spans="1:27" s="9" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="87"/>
-      <c r="B43" s="75"/>
-      <c r="C43" s="75"/>
-      <c r="D43" s="88"/>
+      <c r="A43" s="33"/>
+      <c r="B43" s="34"/>
+      <c r="C43" s="34"/>
+      <c r="D43" s="35"/>
       <c r="E43" s="13"/>
-      <c r="F43" s="89"/>
-      <c r="G43" s="90"/>
+      <c r="F43" s="36"/>
+      <c r="G43" s="37"/>
       <c r="H43" s="14"/>
       <c r="I43" s="14"/>
     </row>
     <row r="44" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="102"/>
-      <c r="B44" s="103"/>
-      <c r="C44" s="103"/>
-      <c r="D44" s="103"/>
-      <c r="E44" s="103"/>
-      <c r="F44" s="103"/>
-      <c r="G44" s="23"/>
-      <c r="H44" s="54"/>
-      <c r="I44" s="104"/>
+      <c r="A44" s="38"/>
+      <c r="B44" s="39"/>
+      <c r="C44" s="39"/>
+      <c r="D44" s="39"/>
+      <c r="E44" s="39"/>
+      <c r="F44" s="39"/>
+      <c r="G44" s="40"/>
+      <c r="H44" s="25"/>
+      <c r="I44" s="41"/>
     </row>
     <row r="45" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="105" t="s">
+      <c r="A45" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="B45" s="61"/>
-      <c r="C45" s="61"/>
-      <c r="D45" s="61"/>
-      <c r="E45" s="106"/>
+      <c r="B45" s="43"/>
+      <c r="C45" s="43"/>
+      <c r="D45" s="43"/>
+      <c r="E45" s="44"/>
       <c r="F45" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="G45" s="107" t="s">
+      <c r="G45" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="H45" s="108"/>
-      <c r="I45" s="108"/>
+      <c r="H45" s="47"/>
+      <c r="I45" s="47"/>
     </row>
     <row r="46" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="53"/>
-      <c r="B46" s="54"/>
-      <c r="C46" s="54"/>
-      <c r="D46" s="54"/>
-      <c r="E46" s="106"/>
+      <c r="A46" s="45"/>
+      <c r="B46" s="25"/>
+      <c r="C46" s="25"/>
+      <c r="D46" s="25"/>
+      <c r="E46" s="44"/>
       <c r="F46" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="G46" s="109" t="s">
+      <c r="G46" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="H46" s="110"/>
-      <c r="I46" s="111"/>
+      <c r="H46" s="49"/>
+      <c r="I46" s="50"/>
     </row>
     <row r="47" spans="1:27" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="47" t="s">
+      <c r="A47" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="B47" s="47"/>
-      <c r="C47" s="47"/>
-      <c r="D47" s="47"/>
-      <c r="E47" s="47"/>
-      <c r="F47" s="47"/>
-      <c r="G47" s="47"/>
-      <c r="H47" s="47"/>
-      <c r="I47" s="91"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="19"/>
+      <c r="G47" s="19"/>
+      <c r="H47" s="19"/>
+      <c r="I47" s="20"/>
       <c r="J47" s="6"/>
       <c r="K47" s="6"/>
       <c r="L47" s="6"/>
@@ -2058,28 +2058,28 @@
       <c r="AA47" s="6"/>
     </row>
     <row r="48" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="34"/>
-      <c r="B48" s="92"/>
-      <c r="C48" s="92"/>
-      <c r="D48" s="92"/>
-      <c r="E48" s="92"/>
-      <c r="F48" s="92"/>
-      <c r="G48" s="92"/>
-      <c r="H48" s="92"/>
-      <c r="I48" s="93"/>
+      <c r="A48" s="21"/>
+      <c r="B48" s="22"/>
+      <c r="C48" s="22"/>
+      <c r="D48" s="22"/>
+      <c r="E48" s="22"/>
+      <c r="F48" s="22"/>
+      <c r="G48" s="22"/>
+      <c r="H48" s="22"/>
+      <c r="I48" s="23"/>
     </row>
     <row r="49" spans="1:27" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="94" t="s">
+      <c r="A49" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="B49" s="54"/>
-      <c r="C49" s="54"/>
-      <c r="D49" s="54"/>
-      <c r="E49" s="54"/>
-      <c r="F49" s="54"/>
-      <c r="G49" s="54"/>
-      <c r="H49" s="54"/>
-      <c r="I49" s="95"/>
+      <c r="B49" s="25"/>
+      <c r="C49" s="25"/>
+      <c r="D49" s="25"/>
+      <c r="E49" s="25"/>
+      <c r="F49" s="25"/>
+      <c r="G49" s="25"/>
+      <c r="H49" s="25"/>
+      <c r="I49" s="26"/>
       <c r="J49" s="6"/>
       <c r="K49" s="6"/>
       <c r="L49" s="6"/>
@@ -2100,29 +2100,90 @@
       <c r="AA49" s="6"/>
     </row>
     <row r="50" spans="1:27" s="9" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="96"/>
-      <c r="B50" s="97"/>
-      <c r="C50" s="97"/>
-      <c r="D50" s="97"/>
-      <c r="E50" s="97"/>
-      <c r="F50" s="97"/>
-      <c r="G50" s="97"/>
-      <c r="H50" s="97"/>
-      <c r="I50" s="98"/>
+      <c r="A50" s="27"/>
+      <c r="B50" s="28"/>
+      <c r="C50" s="28"/>
+      <c r="D50" s="28"/>
+      <c r="E50" s="28"/>
+      <c r="F50" s="28"/>
+      <c r="G50" s="28"/>
+      <c r="H50" s="28"/>
+      <c r="I50" s="29"/>
     </row>
     <row r="51" spans="1:27" s="9" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="99"/>
-      <c r="B51" s="100"/>
-      <c r="C51" s="100"/>
-      <c r="D51" s="100"/>
-      <c r="E51" s="100"/>
-      <c r="F51" s="100"/>
-      <c r="G51" s="100"/>
-      <c r="H51" s="100"/>
-      <c r="I51" s="101"/>
+      <c r="A51" s="30"/>
+      <c r="B51" s="31"/>
+      <c r="C51" s="31"/>
+      <c r="D51" s="31"/>
+      <c r="E51" s="31"/>
+      <c r="F51" s="31"/>
+      <c r="G51" s="31"/>
+      <c r="H51" s="31"/>
+      <c r="I51" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="71">
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="B1:F2"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="B3:F4"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="A5:I5"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:E8"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="A9:I9"/>
+    <mergeCell ref="A10:I11"/>
+    <mergeCell ref="A12:I12"/>
+    <mergeCell ref="A13:E14"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="A16:I19"/>
+    <mergeCell ref="A20:I20"/>
+    <mergeCell ref="A21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G21:I22"/>
+    <mergeCell ref="B23:I23"/>
+    <mergeCell ref="B24:I24"/>
+    <mergeCell ref="B25:I25"/>
+    <mergeCell ref="B26:I26"/>
+    <mergeCell ref="B27:I27"/>
+    <mergeCell ref="B28:I28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:I29"/>
+    <mergeCell ref="A30:I30"/>
+    <mergeCell ref="A31:I31"/>
+    <mergeCell ref="A32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="F32:G33"/>
+    <mergeCell ref="H32:H33"/>
+    <mergeCell ref="I32:I33"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="F42:G42"/>
     <mergeCell ref="A47:I47"/>
     <mergeCell ref="A48:I48"/>
     <mergeCell ref="A49:I49"/>
@@ -2133,67 +2194,6 @@
     <mergeCell ref="A45:E46"/>
     <mergeCell ref="G45:I45"/>
     <mergeCell ref="G46:I46"/>
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="A41:D41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="A37:D37"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="A38:D38"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="A39:D39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="A32:D33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="F32:G33"/>
-    <mergeCell ref="H32:H33"/>
-    <mergeCell ref="I32:I33"/>
-    <mergeCell ref="B28:I28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:I29"/>
-    <mergeCell ref="A30:I30"/>
-    <mergeCell ref="A31:I31"/>
-    <mergeCell ref="B23:I23"/>
-    <mergeCell ref="B24:I24"/>
-    <mergeCell ref="B25:I25"/>
-    <mergeCell ref="B26:I26"/>
-    <mergeCell ref="B27:I27"/>
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="A16:I19"/>
-    <mergeCell ref="A20:I20"/>
-    <mergeCell ref="A21:E22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="G21:I22"/>
-    <mergeCell ref="A9:I9"/>
-    <mergeCell ref="A10:I11"/>
-    <mergeCell ref="A12:I12"/>
-    <mergeCell ref="A13:E14"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="A5:I5"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:E8"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="B1:F2"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="B3:F4"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>